<commit_message>
home commit 30 aug solved sqa no notes issue
</commit_message>
<xml_diff>
--- a/LOGS/89310a5f-45fc-4d11-bcc1-661a581e3891/main_page_service_output/main_pages.xlsx
+++ b/LOGS/89310a5f-45fc-4d11-bcc1-661a581e3891/main_page_service_output/main_pages.xlsx
@@ -1035,10 +1035,10 @@
         <v>190004</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1314,7 +1314,7 @@
         <v>55</v>
       </c>
       <c r="F34" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1331,7 +1331,7 @@
         <v>55</v>
       </c>
       <c r="F35" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:6">

</xml_diff>